<commit_message>
adding new practice scenarios
</commit_message>
<xml_diff>
--- a/SeleniumJavaDemo/Excel/AssignData.xlsx
+++ b/SeleniumJavaDemo/Excel/AssignData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16365" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19380" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>automationuser1983@gmail.com</t>
   </si>
@@ -32,16 +32,27 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>automationuser1982@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,13 +75,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,7 +386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -389,8 +405,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>123456</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -413,8 +429,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>